<commit_message>
Integração com o RocketChat
</commit_message>
<xml_diff>
--- a/Backlog FInal.xlsx
+++ b/Backlog FInal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t xml:space="preserve">5d8b8495a3b6d91aac6c4ef7</t>
   </si>
@@ -31,13 +31,16 @@
     <t xml:space="preserve">Troca de modem</t>
   </si>
   <si>
-    <t xml:space="preserve">5d8b8497a3b6d91aac6c4ef9</t>
+    <t xml:space="preserve">5d8b9238da09856b00edc278</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5d8b9232da09856b00edc270</t>
   </si>
   <si>
     <t xml:space="preserve">5d825b88b6c09ea9e6d9c732</t>
   </si>
   <si>
-    <t xml:space="preserve">5d8b9238da09856b00edc278</t>
+    <t xml:space="preserve">5d8b9237da09856b00edc276 </t>
   </si>
 </sst>
 </file>
@@ -122,7 +125,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -133,6 +136,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -156,18 +163,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -181,7 +188,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="n">
-        <v>43780</v>
+        <v>43791</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -189,32 +196,43 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>43782</v>
-      </c>
+        <v>43793.5833333333</v>
+      </c>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>1</v>
-      </c>
       <c r="C3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>43783.5833333333</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>43791.5833333333</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="1"/>
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>43791.5833333333</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="1"/>
@@ -227,11 +245,9 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="1"/>
-      <c r="G9" s="3"/>
-    </row>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>